<commit_message>
Commiting very nearly final data for data paper I submission for review on Tuesday
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Entoprocta.xlsx
+++ b/data/dataPaper-I-in/arphified/Entoprocta.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="218">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -603,55 +603,19 @@
     <t>source</t>
   </si>
   <si>
-    <t>${gbifOccurrenceID}</t>
-  </si>
-  <si>
-    <t>${catalogNumber}</t>
-  </si>
-  <si>
-    <t>${recordedBy}</t>
-  </si>
-  <si>
-    <t>${individualCount}</t>
-  </si>
-  <si>
-    <t>${sex}</t>
+    <t>imerss.org:PMLS:490</t>
+  </si>
+  <si>
+    <t>Andy Lamb</t>
   </si>
   <si>
     <t>PRESENT</t>
   </si>
   <si>
-    <t>${taxonName}</t>
-  </si>
-  <si>
-    <t>!references.ref</t>
-  </si>
-  <si>
-    <t>iNaturalist:${iNaturalistTaxonId}</t>
-  </si>
-  <si>
-    <t>${summary.taxonName}</t>
-  </si>
-  <si>
-    <t>${kingdom}</t>
-  </si>
-  <si>
-    <t>${phylum}</t>
-  </si>
-  <si>
-    <t>${class}</t>
-  </si>
-  <si>
-    <t>${order}</t>
-  </si>
-  <si>
-    <t>${family}</t>
-  </si>
-  <si>
-    <t>${genus}</t>
-  </si>
-  <si>
-    <t>${summary.authority}</t>
+    <t>Barentsia sp.</t>
+  </si>
+  <si>
+    <t>iNaturalist:211513</t>
   </si>
   <si>
     <t>Galiano Island</t>
@@ -666,61 +630,37 @@
     <t>British Columbia</t>
   </si>
   <si>
-    <t>${locality}</t>
-  </si>
-  <si>
-    <t>${depth}</t>
-  </si>
-  <si>
-    <t>${latitude}</t>
-  </si>
-  <si>
-    <t>${longitude}</t>
-  </si>
-  <si>
-    <t>${coordinateUncertaintyInMeters}</t>
-  </si>
-  <si>
-    <t>Confidence: ${confidence}</t>
-  </si>
-  <si>
-    <t>!references.samplingProtocol</t>
-  </si>
-  <si>
-    <t>!Date:YYYY-MM-DD</t>
-  </si>
-  <si>
-    <t>!Date:HH:mm:ss</t>
-  </si>
-  <si>
-    <t>!Date:YYYY</t>
-  </si>
-  <si>
-    <t>!Date:M</t>
-  </si>
-  <si>
-    <t>!Date:D</t>
-  </si>
-  <si>
-    <t>${fieldNumber}</t>
-  </si>
-  <si>
-    <t>${fieldNotes}</t>
-  </si>
-  <si>
-    <t>${eventRemarks}</t>
-  </si>
-  <si>
-    <t>!references.institutionCode</t>
-  </si>
-  <si>
-    <t>!references.collectionCode</t>
-  </si>
-  <si>
-    <t>!references.datasetName</t>
-  </si>
-  <si>
-    <t>!references.basisOfRecord</t>
+    <t>Alcala Point</t>
+  </si>
+  <si>
+    <t>49.002312</t>
+  </si>
+  <si>
+    <t>-123.590188</t>
+  </si>
+  <si>
+    <t>1985-12-07</t>
+  </si>
+  <si>
+    <t>13:05:00</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>PMLS</t>
+  </si>
+  <si>
+    <t>Pacific Marine Life Survey Dive Records</t>
+  </si>
+  <si>
+    <t>HumanObservation</t>
   </si>
   <si>
     <t>Link type</t>
@@ -1800,451 +1740,451 @@
         <v>196</v>
       </c>
       <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
         <v>197</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
         <v>198</v>
       </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
         <v>199</v>
       </c>
-      <c r="J2" t="s">
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
         <v>200</v>
       </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
         <v>201</v>
       </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="BJ2" t="s">
         <v>202</v>
       </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="BK2" t="s">
         <v>203</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="BL2" t="s">
         <v>204</v>
       </c>
-      <c r="Y2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="BM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO2" t="s">
         <v>205</v>
       </c>
-      <c r="AG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
+      <c r="BP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2">
+        <v>70</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
         <v>206</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="CG2" t="s">
         <v>207</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="CH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI2">
+        <v>500</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>197</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
         <v>208</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="DV2" t="s">
         <v>209</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="DW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY2" t="s">
         <v>210</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="DZ2" t="s">
         <v>211</v>
       </c>
-      <c r="AS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="EA2" t="s">
         <v>212</v>
       </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
+      <c r="EB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
         <v>213</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="ER2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ES2" t="s">
         <v>214</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="ET2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EU2" t="s">
         <v>215</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>216</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>217</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>218</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>219</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>220</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>221</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>198</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>222</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>223</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>224</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>225</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>226</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>227</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>228</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>229</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>230</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>231</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>203</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>232</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>233</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>234</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>235</v>
       </c>
       <c r="EV2" t="s">
         <v>36</v>
@@ -2275,10 +2215,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>